<commit_message>
Update URL short name
</commit_message>
<xml_diff>
--- a/XX_Url/Build_URL.xlsx
+++ b/XX_Url/Build_URL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/Scrapping_git/XX_Url/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/00_Sprint/00_Scrapping_code/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8044C91-AB79-440F-908D-B5A30B03CD08}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607BEFD1-CC35-4D65-AB7D-4C221F794126}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="108">
   <si>
     <t>Linea</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>Homologo Mansfield</t>
+  </si>
+  <si>
+    <t>Mansfield Quantum ADA REAR EL Bowl</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,6 +706,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +907,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,6 +974,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1327,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1355,7 @@
     <col min="8" max="8" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" style="23" customWidth="1"/>
     <col min="10" max="10" width="70.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="85.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.42578125" style="14"/>
   </cols>
@@ -1835,8 +1847,8 @@
       <c r="J13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>94</v>
+      <c r="K13" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>23</v>

</xml_diff>